<commit_message>
added chunked corpuses; trashed incomplete encounter-only corpus; started creating unified ledger to facilitate per-chapter knowledge accumulation
</commit_message>
<xml_diff>
--- a/mallet/30_AM.xlsx
+++ b/mallet/30_AM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apovzner\Documents\Hakluyt\mallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC1064E-F9A7-43D1-930D-30EE4B298090}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C5617B-D1A5-4905-AA73-EDA1556BC7B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26970" windowHeight="10695" xr2:uid="{468B4E7C-0EDA-419C-AC8A-BFE265156530}"/>
   </bookViews>
@@ -1606,7 +1606,7 @@
   <dimension ref="A1:AF590"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>